<commit_message>
combined with workflow engine
</commit_message>
<xml_diff>
--- a/sitedb/test_data/newsite.xlsx
+++ b/sitedb/test_data/newsite.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Project\005 VHA Macro site workflow\Django-Workflow\example data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Project\005 VHA Macro site workflow\Django-Workflow\sitedb\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF50F4DD-C639-465C-8EDB-25F188A0831F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108AF17E-E890-4534-8E78-494535F5728C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>